<commit_message>
Fixed HTML files DME
Updated context and relabeled mislabeled HTML files
</commit_message>
<xml_diff>
--- a/mechanical_turk/HTML_files/Context_DME.xlsx
+++ b/mechanical_turk/HTML_files/Context_DME.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Capstone\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Documents\GitHub\ARL\mechanical_turk\HTML_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E470C918-89E6-4B9C-8B38-44E3B3727FCB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C4D40E-DCED-4906-8AC5-88A209FAE193}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" xr2:uid="{34AA2015-C1CD-4D57-A63D-3DF716DC3691}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Identifier</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Upon meeting the commander of the Chinese team for the first time, he looks slightly discouraged when he sees your rank. You explain that you have taken the place of your commander because he had unexpected business come up. You have been searching a set buildings for natural disaster survivors. He indicates that he wants to search the buildings you have just cleared. He has insited twice that he needs to check the buildings again. You realize you cannot convice him to continue.</t>
+  </si>
+  <si>
+    <t>Upon meeting the commander of the Chinese team for the first time, he looks slightly discouraged when he sees your rank. You explain that you have taken the place of your commander because he had unexpected business come up. He has proposed to set up two aid stations to help victims of a natural distaster, one American and one Chinese. You think it would be better to have one large American aid station, so you ask what benefit his plan has.</t>
   </si>
 </sst>
 </file>
@@ -427,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5143391C-0245-4147-9911-D330566057DB}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -547,7 +550,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -555,7 +558,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -571,6 +574,14 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>